<commit_message>
added dbv control settings to epanet model
</commit_message>
<xml_diff>
--- a/data/devices/flow_device_database.xlsx
+++ b/data/devices/flow_device_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bradw\workspace\FieldLab\data\infradb2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bradw\workspace\bayesian-wq-calibration\data\devices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2803F554-641A-485C-832B-4C88C223DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E156C-A47B-4D39-9D23-F7EE006ED964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-3540" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flow_device_database" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Stoke Lane TS-RT</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>2005_2296</t>
+  </si>
+  <si>
+    <t>620104099_2</t>
+  </si>
+  <si>
+    <t>644926906_2</t>
+  </si>
+  <si>
+    <t>623990497_2</t>
+  </si>
+  <si>
+    <t>612058339_1</t>
   </si>
 </sst>
 </file>
@@ -1114,28 +1126,28 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="12.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.1328125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="12.265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" style="1" customWidth="1"/>
     <col min="12" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="10.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="25.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.3984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="25.73046875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1328125" style="1" customWidth="1"/>
     <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1185,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
@@ -1200,8 +1212,8 @@
       <c r="I2" s="2">
         <v>2297</v>
       </c>
-      <c r="J2" s="2">
-        <v>660167721</v>
+      <c r="J2" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="K2" s="1">
         <v>363600.69400000002</v>
@@ -1210,7 +1222,7 @@
         <v>178807.23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -1237,8 +1249,8 @@
       <c r="I3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="2">
-        <v>672922316</v>
+      <c r="J3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="K3" s="1">
         <v>365517.49200000003</v>
@@ -1247,7 +1259,7 @@
         <v>176035.78700000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>2302</v>
       </c>
       <c r="J4" s="2">
-        <v>617265191</v>
+        <v>579829886</v>
       </c>
       <c r="K4" s="1">
         <v>364021.24099999998</v>
@@ -1284,7 +1296,7 @@
         <v>176683.71599999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>55</v>
       </c>
@@ -1311,8 +1323,8 @@
       <c r="I5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="2">
-        <v>660167748</v>
+      <c r="J5" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="K5" s="1">
         <v>363823.52399999998</v>
@@ -1321,7 +1333,7 @@
         <v>177270.32199999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -1349,7 +1361,7 @@
         <v>61</v>
       </c>
       <c r="J6" s="2">
-        <v>660167766</v>
+        <v>623990697</v>
       </c>
       <c r="K6" s="1">
         <v>364550.14199999999</v>
@@ -1358,7 +1370,7 @@
         <v>176793.28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1385,8 +1397,8 @@
       <c r="I7" s="2">
         <v>2297</v>
       </c>
-      <c r="J7" s="2">
-        <v>612058339</v>
+      <c r="J7" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="K7" s="1">
         <v>363528.038</v>
@@ -1395,7 +1407,7 @@
         <v>179804.54199999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1422,8 +1434,8 @@
       <c r="I8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="2">
-        <v>672922316</v>
+      <c r="J8" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="K8" s="1">
         <v>365519.36200000002</v>
@@ -1432,7 +1444,7 @@
         <v>176037.65900000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1460,7 +1472,7 @@
         <v>2297</v>
       </c>
       <c r="J9" s="2">
-        <v>9554802</v>
+        <v>733663782</v>
       </c>
       <c r="K9" s="1">
         <v>363534.853</v>
@@ -1469,7 +1481,7 @@
         <v>179221.57800000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>175967.54199999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -1541,7 +1553,7 @@
         <v>177970.15400000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1577,7 +1589,7 @@
         <v>175689.96100000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1613,7 +1625,7 @@
         <v>178017.48499999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1652,7 @@
         <v>2302</v>
       </c>
       <c r="J14" s="2">
-        <v>617265191</v>
+        <v>579829886</v>
       </c>
       <c r="K14" s="1">
         <v>364020.88500000001</v>
@@ -1649,7 +1661,7 @@
         <v>176683.56400000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1685,7 +1697,7 @@
         <v>177303.11499999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1711,9 +1723,6 @@
       <c r="H16" s="2">
         <v>2296</v>
       </c>
-      <c r="J16" s="2">
-        <v>660167721</v>
-      </c>
       <c r="K16" s="1">
         <v>363600.59100000001</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>178809.598</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -1747,8 +1756,8 @@
       <c r="I17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="2">
-        <v>660167748</v>
+      <c r="J17" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="K17" s="1">
         <v>363826.19799999997</v>
@@ -1757,7 +1766,7 @@
         <v>177267.19</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>61</v>
       </c>
       <c r="J18" s="2">
-        <v>660167766</v>
+        <v>623990697</v>
       </c>
       <c r="K18" s="1">
         <v>364554</v>
@@ -1793,7 +1802,7 @@
         <v>176791.21299999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1829,7 +1838,7 @@
         <v>179264.10399999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
@@ -1865,7 +1874,7 @@
         <v>177823.649</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>